<commit_message>
up to lt surge
</commit_message>
<xml_diff>
--- a/firered-nettux-new-mons.xlsx
+++ b/firered-nettux-new-mons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\pokefirered-expansion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F37B85-07E2-40E4-B65A-4F7DC5C3B5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E220EC-A2EE-4BBB-949F-1F33A3D15A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="3885" windowWidth="26655" windowHeight="11385" xr2:uid="{4D0F1F34-F3E4-433F-B9BC-51AD106AAB02}"/>
+    <workbookView xWindow="645" yWindow="1635" windowWidth="26655" windowHeight="11385" xr2:uid="{4D0F1F34-F3E4-433F-B9BC-51AD106AAB02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="266">
   <si>
     <t>Sandshrew</t>
   </si>
@@ -725,9 +725,6 @@
     <t>MtMoon_B1F, MtMoon_B2F</t>
   </si>
   <si>
-    <t>Route 3, MtMoon_B2F</t>
-  </si>
-  <si>
     <t>Route 1, MtMoon_B1F</t>
   </si>
   <si>
@@ -753,6 +750,90 @@
   </si>
   <si>
     <t>Route 24, Route 25</t>
+  </si>
+  <si>
+    <t>Wingull</t>
+  </si>
+  <si>
+    <t>Pelipper</t>
+  </si>
+  <si>
+    <t>Rotom</t>
+  </si>
+  <si>
+    <t>Geodude Alola</t>
+  </si>
+  <si>
+    <t>Graveler Alola</t>
+  </si>
+  <si>
+    <t>Golem Alola</t>
+  </si>
+  <si>
+    <t>All Starters</t>
+  </si>
+  <si>
+    <t>Miltank</t>
+  </si>
+  <si>
+    <t>Stantler</t>
+  </si>
+  <si>
+    <t>Chinchou</t>
+  </si>
+  <si>
+    <t>Lantern</t>
+  </si>
+  <si>
+    <t>Route 5</t>
+  </si>
+  <si>
+    <t>Route 4, Route 5</t>
+  </si>
+  <si>
+    <t>Route 24,Route 5</t>
+  </si>
+  <si>
+    <t>Route 3, MtMoon_B2F, Route 6</t>
+  </si>
+  <si>
+    <t>Route 5, Route 6</t>
+  </si>
+  <si>
+    <t>Route 2, Route 6</t>
+  </si>
+  <si>
+    <t>Route 6</t>
+  </si>
+  <si>
+    <t>Route 3, Route 6</t>
+  </si>
+  <si>
+    <t>Route 4, Route 6</t>
+  </si>
+  <si>
+    <t>Route 6, Route 11</t>
+  </si>
+  <si>
+    <t>Route 11</t>
+  </si>
+  <si>
+    <t>Route 4, Route 11</t>
+  </si>
+  <si>
+    <t>Route 4, Route 5, Route 11</t>
+  </si>
+  <si>
+    <t>DiglettsCave_B1F</t>
+  </si>
+  <si>
+    <t>MtMoon_1F, DiglettsCave_B1F</t>
+  </si>
+  <si>
+    <t>MtMoon_B2F,DiglettsCave_B1F</t>
+  </si>
+  <si>
+    <t>Route 11, DiglettsCave_B1F</t>
   </si>
 </sst>
 </file>
@@ -1133,16 +1214,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D266181C-CB66-47C1-88A5-38F785E7523D}">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="G185" sqref="G185"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="G222" sqref="G222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1173,7 +1254,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1271,7 +1352,7 @@
         <v>208</v>
       </c>
       <c r="B24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1310,7 +1391,7 @@
         <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1323,7 +1404,7 @@
         <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1416,7 +1497,7 @@
         <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,7 +1520,7 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1465,7 +1546,7 @@
         <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1485,6 +1566,9 @@
       <c r="A58" t="s">
         <v>35</v>
       </c>
+      <c r="B58" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1499,7 +1583,7 @@
         <v>114</v>
       </c>
       <c r="B60" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1604,7 @@
         <v>115</v>
       </c>
       <c r="B63" t="s">
-        <v>232</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1569,6 +1653,9 @@
       <c r="A70" t="s">
         <v>40</v>
       </c>
+      <c r="B70" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -1600,6 +1687,9 @@
       <c r="A75" t="s">
         <v>135</v>
       </c>
+      <c r="B75" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -1618,10 +1708,10 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B79" t="s">
-        <v>227</v>
+        <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1634,7 +1724,7 @@
         <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,6 +1736,9 @@
       <c r="A83" t="s">
         <v>138</v>
       </c>
+      <c r="B83" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -1656,6 +1749,9 @@
       <c r="A85" t="s">
         <v>139</v>
       </c>
+      <c r="B85" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -1672,7 +1768,7 @@
         <v>142</v>
       </c>
       <c r="B88" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1705,6 +1801,9 @@
       <c r="A93" t="s">
         <v>48</v>
       </c>
+      <c r="B93" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
@@ -1736,6 +1835,9 @@
       <c r="A98" t="s">
         <v>50</v>
       </c>
+      <c r="B98" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -1808,6 +1910,9 @@
       <c r="A110" t="s">
         <v>55</v>
       </c>
+      <c r="B110" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
@@ -1867,6 +1972,9 @@
       <c r="A120" t="s">
         <v>159</v>
       </c>
+      <c r="B120" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
@@ -1955,7 +2063,7 @@
         <v>168</v>
       </c>
       <c r="B135" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -1973,7 +2081,7 @@
         <v>214</v>
       </c>
       <c r="B138" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -1985,11 +2093,17 @@
       <c r="A140" t="s">
         <v>68</v>
       </c>
+      <c r="B140" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>169</v>
       </c>
+      <c r="B141" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
@@ -2008,6 +2122,9 @@
       <c r="A144" t="s">
         <v>171</v>
       </c>
+      <c r="B144" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
@@ -2062,7 +2179,7 @@
         <v>176</v>
       </c>
       <c r="B154" t="s">
-        <v>219</v>
+        <v>256</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -2082,6 +2199,9 @@
       <c r="A157" t="s">
         <v>76</v>
       </c>
+      <c r="B157" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
@@ -2096,7 +2216,7 @@
         <v>179</v>
       </c>
       <c r="B159" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2109,7 +2229,7 @@
         <v>180</v>
       </c>
       <c r="B161" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -2122,7 +2242,7 @@
         <v>181</v>
       </c>
       <c r="B163" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,7 +2265,7 @@
         <v>183</v>
       </c>
       <c r="B167" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -2166,7 +2286,7 @@
         <v>184</v>
       </c>
       <c r="B170" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,7 +2299,7 @@
         <v>186</v>
       </c>
       <c r="B172" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -2199,6 +2319,9 @@
       <c r="A175" t="s">
         <v>188</v>
       </c>
+      <c r="B175" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
@@ -2209,6 +2332,9 @@
       <c r="A177" t="s">
         <v>85</v>
       </c>
+      <c r="B177" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
@@ -2228,7 +2354,7 @@
         <v>190</v>
       </c>
       <c r="B180" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -2241,7 +2367,7 @@
         <v>191</v>
       </c>
       <c r="B182" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,7 +2398,7 @@
         <v>194</v>
       </c>
       <c r="B187" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -2299,6 +2425,9 @@
       <c r="A192" t="s">
         <v>196</v>
       </c>
+      <c r="B192" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
@@ -2395,6 +2524,9 @@
       <c r="A210" t="s">
         <v>99</v>
       </c>
+      <c r="B210" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
@@ -2408,18 +2540,88 @@
       <c r="A212" t="s">
         <v>100</v>
       </c>
+      <c r="B212" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B213" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>238</v>
+      </c>
+      <c r="B215" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>241</v>
+      </c>
+      <c r="B218" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>242</v>
+      </c>
+      <c r="B219" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>245</v>
+      </c>
+      <c r="B221" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>